<commit_message>
change rus to eng in json
</commit_message>
<xml_diff>
--- a/madrich/formats/excel/output2.xlsx
+++ b/madrich/formats/excel/output2.xlsx
@@ -489,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>55.7212478741008</v>
+        <v>55.68444453800417</v>
       </c>
       <c r="C2" t="n">
-        <v>37.66456562948255</v>
+        <v>37.57553578589383</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -529,10 +529,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>55.65442824440024</v>
+        <v>55.67948788095391</v>
       </c>
       <c r="C3" t="n">
-        <v>37.57775449872659</v>
+        <v>37.73522421131663</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -569,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>55.77589785940723</v>
+        <v>55.70251682158581</v>
       </c>
       <c r="C4" t="n">
-        <v>37.66501372019786</v>
+        <v>37.59679890499072</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -609,10 +609,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>55.80969387372262</v>
+        <v>55.67450824280149</v>
       </c>
       <c r="C5" t="n">
-        <v>37.61441964834707</v>
+        <v>37.67161683292756</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -649,10 +649,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>55.66127884311118</v>
+        <v>55.71201203249306</v>
       </c>
       <c r="C6" t="n">
-        <v>37.72465422382138</v>
+        <v>37.56095890833359</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -689,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>55.71044310149883</v>
+        <v>55.71002716873189</v>
       </c>
       <c r="C7" t="n">
-        <v>37.65100651950657</v>
+        <v>37.57445901435683</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -729,10 +729,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>55.80493818701832</v>
+        <v>55.74307564965378</v>
       </c>
       <c r="C8" t="n">
-        <v>37.73763534907381</v>
+        <v>37.67353730835671</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -769,10 +769,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>55.76867706303025</v>
+        <v>55.70794586738244</v>
       </c>
       <c r="C9" t="n">
-        <v>37.66580801798965</v>
+        <v>37.5155211703763</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -809,10 +809,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>55.81244441876391</v>
+        <v>55.70566427688573</v>
       </c>
       <c r="C10" t="n">
-        <v>37.62548680219234</v>
+        <v>37.63377173727263</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -849,10 +849,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>55.74932441886143</v>
+        <v>55.71446251453077</v>
       </c>
       <c r="C11" t="n">
-        <v>37.53066186761053</v>
+        <v>37.73127929139365</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -889,10 +889,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>55.72597658709273</v>
+        <v>55.66529473739025</v>
       </c>
       <c r="C12" t="n">
-        <v>37.73034596188425</v>
+        <v>37.65875383503119</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -929,10 +929,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>55.70830715068415</v>
+        <v>55.76650305010796</v>
       </c>
       <c r="C13" t="n">
-        <v>37.63990179313774</v>
+        <v>37.67643968207631</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -969,10 +969,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>55.79144302693011</v>
+        <v>55.69511294207584</v>
       </c>
       <c r="C14" t="n">
-        <v>37.5618066994403</v>
+        <v>37.73507280763371</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1009,10 +1009,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>55.67489936636758</v>
+        <v>55.66120071251704</v>
       </c>
       <c r="C15" t="n">
-        <v>37.61026407330289</v>
+        <v>37.59824071791409</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1049,10 +1049,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>55.77737994221619</v>
+        <v>55.71691655903573</v>
       </c>
       <c r="C16" t="n">
-        <v>37.4999303654558</v>
+        <v>37.49599886319182</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1089,10 +1089,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>55.7179621959898</v>
+        <v>55.78321235662322</v>
       </c>
       <c r="C17" t="n">
-        <v>37.46202773174195</v>
+        <v>37.55102611159206</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1129,10 +1129,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>55.7533512299203</v>
+        <v>55.75955603165747</v>
       </c>
       <c r="C18" t="n">
-        <v>37.63707170810952</v>
+        <v>37.53418321376897</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1169,10 +1169,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>55.70468398841147</v>
+        <v>55.79916183382227</v>
       </c>
       <c r="C19" t="n">
-        <v>37.5022380006076</v>
+        <v>37.61070137759584</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1209,10 +1209,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>55.81233204471621</v>
+        <v>55.74643952086186</v>
       </c>
       <c r="C20" t="n">
-        <v>37.56076789781397</v>
+        <v>37.50341270110896</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1249,10 +1249,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>55.65952827690968</v>
+        <v>55.8193043852534</v>
       </c>
       <c r="C21" t="n">
-        <v>37.48921221401125</v>
+        <v>37.54766770218015</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1289,10 +1289,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>55.66118283695216</v>
+        <v>55.75559622911472</v>
       </c>
       <c r="C22" t="n">
-        <v>37.47698154613471</v>
+        <v>37.63597152864205</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1329,10 +1329,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>55.68472914612728</v>
+        <v>55.67665421830194</v>
       </c>
       <c r="C23" t="n">
-        <v>37.61884846927232</v>
+        <v>37.68190332216877</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1369,10 +1369,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>55.7010398894577</v>
+        <v>55.72252272070857</v>
       </c>
       <c r="C24" t="n">
-        <v>37.63729299147909</v>
+        <v>37.7341602222447</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1409,10 +1409,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>55.80183324969308</v>
+        <v>55.73990078453081</v>
       </c>
       <c r="C25" t="n">
-        <v>37.52360802653466</v>
+        <v>37.7293620568059</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1449,10 +1449,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>55.74960018177368</v>
+        <v>55.79835675044812</v>
       </c>
       <c r="C26" t="n">
-        <v>37.57526534083051</v>
+        <v>37.45008770291449</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1489,10 +1489,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>55.65514548886041</v>
+        <v>55.65125928042025</v>
       </c>
       <c r="C27" t="n">
-        <v>37.68582316570927</v>
+        <v>37.61993628386446</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1529,10 +1529,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>55.71090946417108</v>
+        <v>55.71478725332855</v>
       </c>
       <c r="C28" t="n">
-        <v>37.46670487755487</v>
+        <v>37.5751873780851</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1569,10 +1569,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>55.7564790810891</v>
+        <v>55.78064293979297</v>
       </c>
       <c r="C29" t="n">
-        <v>37.48473001691821</v>
+        <v>37.55606655974139</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1609,10 +1609,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>55.73578509392343</v>
+        <v>55.68606143474795</v>
       </c>
       <c r="C30" t="n">
-        <v>37.570921816719</v>
+        <v>37.52943375936608</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1649,10 +1649,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>55.78432150960391</v>
+        <v>55.69626062163972</v>
       </c>
       <c r="C31" t="n">
-        <v>37.63205960331921</v>
+        <v>37.6876735666027</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1689,10 +1689,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>55.70910311009364</v>
+        <v>55.75604903038228</v>
       </c>
       <c r="C32" t="n">
-        <v>37.57861259952111</v>
+        <v>37.47946098310879</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1729,10 +1729,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>55.65422197545976</v>
+        <v>55.75183617624158</v>
       </c>
       <c r="C33" t="n">
-        <v>37.73935699120824</v>
+        <v>37.56891589443138</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1769,10 +1769,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>55.72025831113447</v>
+        <v>55.70240577242451</v>
       </c>
       <c r="C34" t="n">
-        <v>37.59356576617923</v>
+        <v>37.6712653294931</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1809,10 +1809,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>55.70454050783694</v>
+        <v>55.75547556771942</v>
       </c>
       <c r="C35" t="n">
-        <v>37.5062132461096</v>
+        <v>37.7326695374279</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1849,10 +1849,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>55.67611946001309</v>
+        <v>55.71823477831779</v>
       </c>
       <c r="C36" t="n">
-        <v>37.74956962916149</v>
+        <v>37.46397928098686</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1889,10 +1889,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>55.71502413146488</v>
+        <v>55.77819091680744</v>
       </c>
       <c r="C37" t="n">
-        <v>37.49688117643391</v>
+        <v>37.63454577765092</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1929,10 +1929,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>55.7882608650455</v>
+        <v>55.66507806523065</v>
       </c>
       <c r="C38" t="n">
-        <v>37.69282545418767</v>
+        <v>37.70267233299501</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1969,10 +1969,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>55.70853325229178</v>
+        <v>55.68996882645116</v>
       </c>
       <c r="C39" t="n">
-        <v>37.74600311470631</v>
+        <v>37.46856778456943</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2009,10 +2009,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>55.74040035065435</v>
+        <v>55.79546550716621</v>
       </c>
       <c r="C40" t="n">
-        <v>37.69530610343202</v>
+        <v>37.55812694306487</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2049,10 +2049,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>55.75266882579015</v>
+        <v>55.74469583208078</v>
       </c>
       <c r="C41" t="n">
-        <v>37.5154295746844</v>
+        <v>37.74482413564305</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -2089,10 +2089,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>55.79089785503592</v>
+        <v>55.77060872411177</v>
       </c>
       <c r="C42" t="n">
-        <v>37.72552965073857</v>
+        <v>37.63068928072016</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2129,10 +2129,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>55.79739424425735</v>
+        <v>55.76808816408723</v>
       </c>
       <c r="C43" t="n">
-        <v>37.65373155782401</v>
+        <v>37.53883926558113</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2169,10 +2169,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>55.74121141137349</v>
+        <v>55.67956458238026</v>
       </c>
       <c r="C44" t="n">
-        <v>37.59342773678498</v>
+        <v>37.58811896900087</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -2209,10 +2209,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>55.6787355828317</v>
+        <v>55.71076548708987</v>
       </c>
       <c r="C45" t="n">
-        <v>37.62358076895724</v>
+        <v>37.68635213515589</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -2249,10 +2249,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>55.81351141371467</v>
+        <v>55.74793554571764</v>
       </c>
       <c r="C46" t="n">
-        <v>37.71398453823698</v>
+        <v>37.69384468198596</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(2020-10-01 10:00:00 - 2020-10-01 18:00:00)</t>
+          <t>(2020-10-01 08:00:00 - 2020-10-01 22:00:00)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>bicycle</t>
+          <t>car</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(2020-10-01 12:00:00 - 2020-10-01 21:00:00)</t>
+          <t>(2020-10-01 08:00:00 - 2020-10-01 19:00:00)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>foot</t>
+          <t>car</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(2020-10-01 08:00:00 - 2020-10-01 20:00:00)</t>
+          <t>(2020-10-01 12:00:00 - 2020-10-01 19:00:00)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2596,14 +2596,14 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>55.68327626783568</v>
+        <v>55.75530405177981</v>
       </c>
       <c r="D2" t="n">
-        <v>37.61122734892008</v>
+        <v>37.46851600393571</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(2020-10-01 12:00:00 - 2020-10-01 20:00:00)</t>
+          <t>(2020-10-01 09:00:00 - 2020-10-01 22:00:00)</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -2620,14 +2620,14 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>55.75912653378755</v>
+        <v>55.68947874064456</v>
       </c>
       <c r="D3" t="n">
-        <v>37.61716594622039</v>
+        <v>37.52911383980694</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(2020-10-01 09:00:00 - 2020-10-01 19:00:00)</t>
+          <t>(2020-10-01 11:00:00 - 2020-10-01 19:00:00)</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -2644,14 +2644,14 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>55.65874708070027</v>
+        <v>55.7771001718272</v>
       </c>
       <c r="D4" t="n">
-        <v>37.59252538371483</v>
+        <v>37.54383200505681</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(2020-10-01 12:00:00 - 2020-10-01 19:00:00)</t>
+          <t>(2020-10-01 10:00:00 - 2020-10-01 21:00:00)</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -2716,12 +2716,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>bicycle</t>
+          <t>car</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>bicycle</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -2748,12 +2748,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>foot</t>
+          <t>car</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>foot</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>

</xml_diff>